<commit_message>
More work on database serialization.
</commit_message>
<xml_diff>
--- a/JPAD-Apps/JPAD_Executable/out/IRON/PERFORMANCE/Performance.xlsx
+++ b/JPAD-Apps/JPAD_Executable/out/IRON/PERFORMANCE/Performance.xlsx
@@ -1039,7 +1039,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>669.2081120749972</v>
+        <v>596.6164669838503</v>
       </c>
     </row>
     <row r="3">
@@ -1050,7 +1050,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>43.85697413706076</v>
+        <v>40.123172629899884</v>
       </c>
     </row>
     <row r="4">
@@ -1061,7 +1061,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>258.88689020443326</v>
+        <v>256.1962580549347</v>
       </c>
     </row>
     <row r="5">
@@ -1072,7 +1072,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>971.9519764164911</v>
+        <v>892.9358976686848</v>
       </c>
     </row>
     <row r="6">
@@ -1083,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>1117.7447728789648</v>
+        <v>1026.8762823189873</v>
       </c>
     </row>
     <row r="7">
@@ -1094,7 +1094,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>1118.0403113059162</v>
+        <v>1074.8076489634022</v>
       </c>
     </row>
     <row r="8">
@@ -1110,7 +1110,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>2195.5646721620647</v>
+        <v>1957.403106902396</v>
       </c>
     </row>
     <row r="10">
@@ -1121,7 +1121,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>143.8877104234277</v>
+        <v>131.63770547867418</v>
       </c>
     </row>
     <row r="11">
@@ -1132,7 +1132,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>849.3664376785869</v>
+        <v>840.538904379707</v>
       </c>
     </row>
     <row r="12">
@@ -1143,7 +1143,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>3188.8188202640786</v>
+        <v>2929.579716760777</v>
       </c>
     </row>
     <row r="13">
@@ -1154,7 +1154,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>3667.14164330369</v>
+        <v>3369.016674274893</v>
       </c>
     </row>
     <row r="14">
@@ -1165,7 +1165,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="n">
-        <v>3668.1112575653424</v>
+        <v>3526.2718141843907</v>
       </c>
     </row>
     <row r="15">
@@ -1192,7 +1192,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>54.295416771801754</v>
+        <v>54.572720025021354</v>
       </c>
     </row>
     <row r="18">
@@ -1214,7 +1214,7 @@
         <v>13</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0</v>
+        <v>61.75510851241276</v>
       </c>
     </row>
     <row r="20">
@@ -1225,7 +1225,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="n">
-        <v>60.39680242724415</v>
+        <v>60.34630984238268</v>
       </c>
     </row>
     <row r="21">
@@ -1236,7 +1236,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="n">
-        <v>66.66323558224724</v>
+        <v>66.7957091363796</v>
       </c>
     </row>
     <row r="22">
@@ -1263,7 +1263,7 @@
         <v>19</v>
       </c>
       <c r="C24" t="n">
-        <v>105.54184685663408</v>
+        <v>106.08088125814086</v>
       </c>
     </row>
     <row r="25">
@@ -1285,7 +1285,7 @@
         <v>19</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0</v>
+        <v>120.04232756192548</v>
       </c>
     </row>
     <row r="27">
@@ -1296,7 +1296,7 @@
         <v>19</v>
       </c>
       <c r="C27" t="n">
-        <v>117.40199175922189</v>
+        <v>117.30384202622983</v>
       </c>
     </row>
     <row r="28">
@@ -1307,7 +1307,7 @@
         <v>19</v>
       </c>
       <c r="C28" t="n">
-        <v>129.58296333482187</v>
+        <v>129.84047132341607</v>
       </c>
     </row>
     <row r="29">
@@ -1323,7 +1323,7 @@
         <v>21</v>
       </c>
       <c r="C30" t="n">
-        <v>0.9701701701702129</v>
+        <v>0.9751251251251685</v>
       </c>
     </row>
     <row r="31">
@@ -1345,7 +1345,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0</v>
+        <v>1.1034626437471822</v>
       </c>
     </row>
     <row r="33">
@@ -1356,7 +1356,7 @@
         <v>21</v>
       </c>
       <c r="C33" t="n">
-        <v>1.0791919387016753</v>
+        <v>1.0782897189092888</v>
       </c>
     </row>
     <row r="34">
@@ -1367,7 +1367,7 @@
         <v>21</v>
       </c>
       <c r="C34" t="n">
-        <v>1.1911628357278676</v>
+        <v>1.1935299211689059</v>
       </c>
     </row>
     <row r="35">
@@ -1383,7 +1383,7 @@
         <v>27</v>
       </c>
       <c r="C36" t="n">
-        <v>26.132964488757466</v>
+        <v>23.43419722937321</v>
       </c>
     </row>
   </sheetData>
@@ -1422,7 +1422,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>13203.564275020875</v>
+        <v>9669.069450859442</v>
       </c>
     </row>
     <row r="3">
@@ -1433,7 +1433,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>43318.78042985851</v>
+        <v>31722.66880203229</v>
       </c>
     </row>
     <row r="4">
@@ -1444,7 +1444,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>12826.851658828022</v>
+        <v>9348.201284686442</v>
       </c>
     </row>
     <row r="5">
@@ -1455,7 +1455,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>42082.84664969823</v>
+        <v>30669.951721412206</v>
       </c>
     </row>
     <row r="6">
@@ -1466,7 +1466,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="n">
-        <v>11.880338748449113</v>
+        <v>17.862603168346723</v>
       </c>
     </row>
     <row r="7">
@@ -1477,7 +1477,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="n">
-        <v>13.15031648311868</v>
+        <v>20.122330859639487</v>
       </c>
     </row>
     <row r="8">
@@ -1488,7 +1488,7 @@
         <v>34</v>
       </c>
       <c r="C8" t="n">
-        <v>539.4938792127734</v>
+        <v>812.6483582153</v>
       </c>
     </row>
     <row r="9">
@@ -1504,7 +1504,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>8899.914409208148</v>
+        <v>6771.713825197039</v>
       </c>
     </row>
     <row r="11">
@@ -1515,7 +1515,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>29199.194255932245</v>
+        <v>22216.908875318368</v>
       </c>
     </row>
     <row r="12">
@@ -1526,7 +1526,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>7743.643862926461</v>
+        <v>6306.196297676666</v>
       </c>
     </row>
     <row r="13">
@@ -1537,7 +1537,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>25405.655718262664</v>
+        <v>20689.62039920166</v>
       </c>
     </row>
   </sheetData>
@@ -1576,7 +1576,7 @@
         <v>38</v>
       </c>
       <c r="C2" t="n">
-        <v>36686.6827639734</v>
+        <v>42000.99711496192</v>
       </c>
     </row>
     <row r="3">
@@ -1587,7 +1587,7 @@
         <v>39</v>
       </c>
       <c r="C3" t="n">
-        <v>8247.494378003223</v>
+        <v>9442.199770548577</v>
       </c>
     </row>
     <row r="4">
@@ -1625,7 +1625,7 @@
         <v>42</v>
       </c>
       <c r="C7" t="n">
-        <v>6674704.453556204</v>
+        <v>7641580.578452785</v>
       </c>
     </row>
     <row r="8">
@@ -1636,7 +1636,7 @@
         <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>9075.06937950453</v>
+        <v>10389.654613334325</v>
       </c>
     </row>
     <row r="9">
@@ -1685,7 +1685,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="n">
-        <v>110.32807237771365</v>
+        <v>106.8707019388792</v>
       </c>
     </row>
     <row r="14">
@@ -1707,7 +1707,7 @@
         <v>19</v>
       </c>
       <c r="C15" t="n">
-        <v>214.4606158530071</v>
+        <v>207.74002536715176</v>
       </c>
     </row>
     <row r="16">
@@ -1734,7 +1734,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="n">
-        <v>180.2301953601185</v>
+        <v>174.58166847582703</v>
       </c>
     </row>
     <row r="19">
@@ -1756,7 +1756,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>350.3394726222606</v>
+        <v>339.3596147478279</v>
       </c>
     </row>
     <row r="21">
@@ -1783,7 +1783,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5943681414445151</v>
+        <v>0.5757397911237961</v>
       </c>
     </row>
     <row r="24">
@@ -1876,7 +1876,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="n">
-        <v>241.74704447949074</v>
+        <v>458.1367252506084</v>
       </c>
     </row>
   </sheetData>
@@ -2221,7 +2221,7 @@
         <v>31</v>
       </c>
       <c r="C3" t="n">
-        <v>329.94661127795257</v>
+        <v>337.8579796310777</v>
       </c>
     </row>
     <row r="4">
@@ -2243,7 +2243,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="n">
-        <v>46258.46413115856</v>
+        <v>45753.3027816041</v>
       </c>
     </row>
     <row r="6">
@@ -2254,7 +2254,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="n">
-        <v>7738.458809306721</v>
+        <v>8270.20759831143</v>
       </c>
     </row>
     <row r="7">
@@ -2265,7 +2265,7 @@
         <v>34</v>
       </c>
       <c r="C7" t="n">
-        <v>7351.535868841385</v>
+        <v>7856.697218395859</v>
       </c>
     </row>
     <row r="8">
@@ -2298,7 +2298,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="n">
-        <v>117.0</v>
+        <v>112.0</v>
       </c>
     </row>
     <row r="11">
@@ -2314,7 +2314,7 @@
         <v>53</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6168655191063858</v>
+        <v>0.5744527793216202</v>
       </c>
     </row>
     <row r="13">
@@ -2325,7 +2325,7 @@
         <v>53</v>
       </c>
       <c r="C13" t="n">
-        <v>67.97815221502468</v>
+        <v>110.31162087361062</v>
       </c>
     </row>
     <row r="14">
@@ -2336,7 +2336,7 @@
         <v>53</v>
       </c>
       <c r="C14" t="n">
-        <v>1375.9067160419193</v>
+        <v>1331.2178207268348</v>
       </c>
     </row>
     <row r="15">
@@ -2347,7 +2347,7 @@
         <v>53</v>
       </c>
       <c r="C15" t="n">
-        <v>95.44884708572283</v>
+        <v>95.44884708572295</v>
       </c>
     </row>
     <row r="16">
@@ -2358,7 +2358,7 @@
         <v>53</v>
       </c>
       <c r="C16" t="n">
-        <v>17.59759933335158</v>
+        <v>19.999451335195772</v>
       </c>
     </row>
     <row r="17">
@@ -2369,7 +2369,7 @@
         <v>53</v>
       </c>
       <c r="C17" t="n">
-        <v>100.0</v>
+        <v>99.99999999999989</v>
       </c>
     </row>
     <row r="18">
@@ -2380,7 +2380,7 @@
         <v>53</v>
       </c>
       <c r="C18" t="n">
-        <v>38.39482262187971</v>
+        <v>38.39482262187994</v>
       </c>
     </row>
     <row r="19">
@@ -2402,7 +2402,7 @@
         <v>53</v>
       </c>
       <c r="C20" t="n">
-        <v>3.5867091019897543</v>
+        <v>3.586709101989527</v>
       </c>
     </row>
     <row r="21">
@@ -2413,7 +2413,7 @@
         <v>53</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4703680489050157</v>
+        <v>0.46664081347523734</v>
       </c>
     </row>
     <row r="22">
@@ -2429,7 +2429,7 @@
         <v>31</v>
       </c>
       <c r="C23" t="n">
-        <v>0.47670509563225444</v>
+        <v>0.4316275459364846</v>
       </c>
     </row>
     <row r="24">
@@ -2440,7 +2440,7 @@
         <v>31</v>
       </c>
       <c r="C24" t="n">
-        <v>16.221226440395874</v>
+        <v>25.575183551726838</v>
       </c>
     </row>
     <row r="25">
@@ -2451,7 +2451,7 @@
         <v>31</v>
       </c>
       <c r="C25" t="n">
-        <v>232.14272456678623</v>
+        <v>230.91840265904682</v>
       </c>
     </row>
     <row r="26">
@@ -2473,7 +2473,7 @@
         <v>31</v>
       </c>
       <c r="C27" t="n">
-        <v>4.921531882155904</v>
+        <v>5.564774653625676</v>
       </c>
     </row>
     <row r="28">
@@ -2484,7 +2484,7 @@
         <v>31</v>
       </c>
       <c r="C28" t="n">
-        <v>16.982020577107875</v>
+        <v>16.167108869887755</v>
       </c>
     </row>
     <row r="29">
@@ -2528,7 +2528,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.2357360492078726</v>
+        <v>0.2342156841876033</v>
       </c>
     </row>
     <row r="33">
@@ -2544,7 +2544,7 @@
         <v>34</v>
       </c>
       <c r="C34" t="n">
-        <v>27.61743452628439</v>
+        <v>25.36704069108756</v>
       </c>
     </row>
     <row r="35">
@@ -2555,7 +2555,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>627.7258121556208</v>
+        <v>981.2000635683705</v>
       </c>
     </row>
     <row r="36">
@@ -2566,7 +2566,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="n">
-        <v>4999.069054438045</v>
+        <v>4854.638646938965</v>
       </c>
     </row>
     <row r="37">
@@ -2577,7 +2577,7 @@
         <v>34</v>
       </c>
       <c r="C37" t="n">
-        <v>233.8459233606768</v>
+        <v>458.10334024339545</v>
       </c>
     </row>
     <row r="38">
@@ -2588,7 +2588,7 @@
         <v>34</v>
       </c>
       <c r="C38" t="n">
-        <v>220.14890825158227</v>
+        <v>267.2715149059618</v>
       </c>
     </row>
     <row r="39">
@@ -2599,7 +2599,7 @@
         <v>34</v>
       </c>
       <c r="C39" t="n">
-        <v>525.612689142094</v>
+        <v>542.4398062829382</v>
       </c>
     </row>
     <row r="40">
@@ -2610,7 +2610,7 @@
         <v>34</v>
       </c>
       <c r="C40" t="n">
-        <v>113.67457037553459</v>
+        <v>127.89008262095149</v>
       </c>
     </row>
     <row r="41">
@@ -2621,7 +2621,7 @@
         <v>34</v>
       </c>
       <c r="C41" t="n">
-        <v>590.1742747941212</v>
+        <v>585.2125436580286</v>
       </c>
     </row>
     <row r="42">
@@ -2632,7 +2632,7 @@
         <v>34</v>
       </c>
       <c r="C42" t="n">
-        <v>13.667201797426515</v>
+        <v>14.57417948615921</v>
       </c>
     </row>
     <row r="43">
@@ -2659,7 +2659,7 @@
         <v>34</v>
       </c>
       <c r="C45" t="n">
-        <v>53582.38256547371</v>
+        <v>53584.6329593089</v>
       </c>
     </row>
     <row r="46">
@@ -2670,7 +2670,7 @@
         <v>34</v>
       </c>
       <c r="C46" t="n">
-        <v>52954.65675331808</v>
+        <v>52603.43289574052</v>
       </c>
     </row>
     <row r="47">
@@ -2681,7 +2681,7 @@
         <v>34</v>
       </c>
       <c r="C47" t="n">
-        <v>47955.58769888003</v>
+        <v>47748.794248801554</v>
       </c>
     </row>
     <row r="48">
@@ -2692,7 +2692,7 @@
         <v>34</v>
       </c>
       <c r="C48" t="n">
-        <v>47721.741775519346</v>
+        <v>47290.69090855816</v>
       </c>
     </row>
     <row r="49">
@@ -2703,7 +2703,7 @@
         <v>34</v>
       </c>
       <c r="C49" t="n">
-        <v>47501.59286726776</v>
+        <v>47023.41939365219</v>
       </c>
     </row>
     <row r="50">
@@ -2714,7 +2714,7 @@
         <v>34</v>
       </c>
       <c r="C50" t="n">
-        <v>46975.98017812567</v>
+        <v>46480.97958736925</v>
       </c>
     </row>
     <row r="51">
@@ -2725,7 +2725,7 @@
         <v>34</v>
       </c>
       <c r="C51" t="n">
-        <v>46862.305607750124</v>
+        <v>46353.0895047483</v>
       </c>
     </row>
     <row r="52">
@@ -2736,7 +2736,7 @@
         <v>34</v>
       </c>
       <c r="C52" t="n">
-        <v>46272.13133295599</v>
+        <v>45767.87696109027</v>
       </c>
     </row>
     <row r="53">
@@ -2747,7 +2747,7 @@
         <v>34</v>
       </c>
       <c r="C53" t="n">
-        <v>46258.464131158566</v>
+        <v>45753.3027816041</v>
       </c>
     </row>
     <row r="54">
@@ -2758,7 +2758,7 @@
         <v>34</v>
       </c>
       <c r="C54" t="n">
-        <v>46258.46413115856</v>
+        <v>45753.3027816041</v>
       </c>
     </row>
     <row r="55">
@@ -2790,7 +2790,7 @@
         <v>19</v>
       </c>
       <c r="C58" t="n">
-        <v>137.26093310715834</v>
+        <v>137.59550397418738</v>
       </c>
     </row>
     <row r="59">
@@ -2812,7 +2812,7 @@
         <v>10</v>
       </c>
       <c r="C60" t="n">
-        <v>0.20753122438118274</v>
+        <v>0.20803707772273483</v>
       </c>
     </row>
     <row r="61">
@@ -2834,7 +2834,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>2.373778178019884</v>
+        <v>2.3607308590365443</v>
       </c>
     </row>
     <row r="63">
@@ -2856,7 +2856,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>0.1679261811384085</v>
+        <v>0.16696125584529825</v>
       </c>
     </row>
     <row r="65">
@@ -2878,7 +2878,7 @@
         <v>10</v>
       </c>
       <c r="C66" t="n">
-        <v>14.135843273082969</v>
+        <v>14.139393280701801</v>
       </c>
     </row>
     <row r="67">
@@ -2889,7 +2889,7 @@
         <v>127</v>
       </c>
       <c r="C67" t="n">
-        <v>42765.581636341776</v>
+        <v>48830.439790029304</v>
       </c>
     </row>
     <row r="68">
@@ -2900,7 +2900,7 @@
         <v>127</v>
       </c>
       <c r="C68" t="n">
-        <v>30333.773857010274</v>
+        <v>30266.30346290084</v>
       </c>
     </row>
     <row r="69">
@@ -2922,7 +2922,7 @@
         <v>127</v>
       </c>
       <c r="C70" t="n">
-        <v>10305.906173978623</v>
+        <v>10296.700202011521</v>
       </c>
     </row>
     <row r="71">
@@ -2987,7 +2987,7 @@
         <v>10</v>
       </c>
       <c r="C77" t="n">
-        <v>0.8551908855885116</v>
+        <v>0.8552268025486152</v>
       </c>
     </row>
     <row r="78">
@@ -2998,7 +2998,7 @@
         <v>10</v>
       </c>
       <c r="C78" t="n">
-        <v>2.2554356529289046</v>
+        <v>2.240476386660221</v>
       </c>
     </row>
     <row r="79">
@@ -3009,7 +3009,7 @@
         <v>10</v>
       </c>
       <c r="C79" t="n">
-        <v>0.04753022442134632</v>
+        <v>0.04753227987684003</v>
       </c>
     </row>
     <row r="80">
@@ -3031,7 +3031,7 @@
         <v>10</v>
       </c>
       <c r="C81" t="n">
-        <v>17.992569906832514</v>
+        <v>17.992547480671593</v>
       </c>
     </row>
     <row r="82">
@@ -3042,7 +3042,7 @@
         <v>10</v>
       </c>
       <c r="C82" t="n">
-        <v>17.87601754279726</v>
+        <v>17.75745414867023</v>
       </c>
     </row>
     <row r="83">
@@ -3053,7 +3053,7 @@
         <v>127</v>
       </c>
       <c r="C83" t="n">
-        <v>22747.1833668971</v>
+        <v>21081.67975315212</v>
       </c>
     </row>
     <row r="84">
@@ -3064,7 +3064,7 @@
         <v>127</v>
       </c>
       <c r="C84" t="n">
-        <v>10802.459853028651</v>
+        <v>8827.371728515536</v>
       </c>
     </row>
     <row r="85">
@@ -3075,7 +3075,7 @@
         <v>127</v>
       </c>
       <c r="C85" t="n">
-        <v>6565.424639538379</v>
+        <v>6565.708589934272</v>
       </c>
     </row>
     <row r="86">
@@ -3086,7 +3086,7 @@
         <v>127</v>
       </c>
       <c r="C86" t="n">
-        <v>6672.143607643273</v>
+        <v>6672.423829427438</v>
       </c>
     </row>
     <row r="87">
@@ -3107,7 +3107,7 @@
         <v>19</v>
       </c>
       <c r="C89" t="n">
-        <v>346.64327055808104</v>
+        <v>336.23970385741416</v>
       </c>
     </row>
     <row r="90">
@@ -3118,7 +3118,7 @@
         <v>19</v>
       </c>
       <c r="C90" t="n">
-        <v>367.02555186050284</v>
+        <v>357.89036943174386</v>
       </c>
     </row>
     <row r="91">
@@ -3129,7 +3129,7 @@
         <v>10</v>
       </c>
       <c r="C91" t="n">
-        <v>0.5880969260101238</v>
+        <v>0.5704467763725632</v>
       </c>
     </row>
     <row r="92">
@@ -3140,7 +3140,7 @@
         <v>10</v>
       </c>
       <c r="C92" t="n">
-        <v>0.6226764433327294</v>
+        <v>0.6071781684167169</v>
       </c>
     </row>
     <row r="93">
@@ -3151,7 +3151,7 @@
         <v>10</v>
       </c>
       <c r="C93" t="n">
-        <v>0.6775979696652159</v>
+        <v>0.715401067700975</v>
       </c>
     </row>
     <row r="94">
@@ -3162,7 +3162,7 @@
         <v>10</v>
       </c>
       <c r="C94" t="n">
-        <v>0.5164820083104917</v>
+        <v>0.5413328491466605</v>
       </c>
     </row>
     <row r="95">
@@ -3173,7 +3173,7 @@
         <v>10</v>
       </c>
       <c r="C95" t="n">
-        <v>0.039211887293051216</v>
+        <v>0.04080740911388062</v>
       </c>
     </row>
     <row r="96">
@@ -3184,7 +3184,7 @@
         <v>10</v>
       </c>
       <c r="C96" t="n">
-        <v>0.033553044220082685</v>
+        <v>0.034303702299842406</v>
       </c>
     </row>
     <row r="97">
@@ -3195,7 +3195,7 @@
         <v>10</v>
       </c>
       <c r="C97" t="n">
-        <v>17.28042225055803</v>
+        <v>17.531156308025242</v>
       </c>
     </row>
     <row r="98">
@@ -3206,7 +3206,7 @@
         <v>10</v>
       </c>
       <c r="C98" t="n">
-        <v>15.39299995919175</v>
+        <v>15.780595470861098</v>
       </c>
     </row>
     <row r="99">
@@ -3217,7 +3217,7 @@
         <v>127</v>
       </c>
       <c r="C99" t="n">
-        <v>6755.913282549102</v>
+        <v>6615.120880290459</v>
       </c>
     </row>
     <row r="100">
@@ -3228,7 +3228,7 @@
         <v>127</v>
       </c>
       <c r="C100" t="n">
-        <v>6480.7505215703095</v>
+        <v>6300.018029145074</v>
       </c>
     </row>
     <row r="101">
@@ -3239,7 +3239,7 @@
         <v>127</v>
       </c>
       <c r="C101" t="n">
-        <v>6755.913282549102</v>
+        <v>6615.120880290459</v>
       </c>
     </row>
     <row r="102">
@@ -3250,7 +3250,7 @@
         <v>127</v>
       </c>
       <c r="C102" t="n">
-        <v>6480.7505215703095</v>
+        <v>6300.018029145074</v>
       </c>
     </row>
     <row r="103">
@@ -3315,7 +3315,7 @@
         <v>10</v>
       </c>
       <c r="C109" t="n">
-        <v>0.5703914497758048</v>
+        <v>0.5679318153212122</v>
       </c>
     </row>
     <row r="110">
@@ -3326,7 +3326,7 @@
         <v>10</v>
       </c>
       <c r="C110" t="n">
-        <v>0.565747853845448</v>
+        <v>0.5567542964326584</v>
       </c>
     </row>
     <row r="111">
@@ -3337,7 +3337,7 @@
         <v>10</v>
       </c>
       <c r="C111" t="n">
-        <v>0.035233312346772176</v>
+        <v>0.03515275498620793</v>
       </c>
     </row>
     <row r="112">
@@ -3348,7 +3348,7 @@
         <v>10</v>
       </c>
       <c r="C112" t="n">
-        <v>0.03508240475341164</v>
+        <v>0.03479270236411694</v>
       </c>
     </row>
     <row r="113">
@@ -3359,7 +3359,7 @@
         <v>10</v>
       </c>
       <c r="C113" t="n">
-        <v>16.188981727347016</v>
+        <v>16.156111108333853</v>
       </c>
     </row>
     <row r="114">
@@ -3370,7 +3370,7 @@
         <v>10</v>
       </c>
       <c r="C114" t="n">
-        <v>16.12625639040411</v>
+        <v>16.00204234227177</v>
       </c>
     </row>
     <row r="115">
@@ -3381,7 +3381,7 @@
         <v>127</v>
       </c>
       <c r="C115" t="n">
-        <v>1921.4569483987661</v>
+        <v>1922.9897727282992</v>
       </c>
     </row>
     <row r="116">
@@ -3392,7 +3392,7 @@
         <v>127</v>
       </c>
       <c r="C116" t="n">
-        <v>-17.184052726102042</v>
+        <v>29.79705069041176</v>
       </c>
     </row>
     <row r="117">
@@ -3403,7 +3403,7 @@
         <v>127</v>
       </c>
       <c r="C117" t="n">
-        <v>6274.9234109860145</v>
+        <v>6259.134734634988</v>
       </c>
     </row>
     <row r="118">
@@ -3414,7 +3414,7 @@
         <v>127</v>
       </c>
       <c r="C118" t="n">
-        <v>6245.115634829497</v>
+        <v>6187.3849557971735</v>
       </c>
     </row>
     <row r="119">
@@ -3479,7 +3479,7 @@
         <v>10</v>
       </c>
       <c r="C125" t="n">
-        <v>0.7616533267196718</v>
+        <v>0.7547736254641989</v>
       </c>
     </row>
     <row r="126">
@@ -3490,7 +3490,7 @@
         <v>10</v>
       </c>
       <c r="C126" t="n">
-        <v>1.152449936078255</v>
+        <v>1.1408488306028572</v>
       </c>
     </row>
     <row r="127">
@@ -3501,7 +3501,7 @@
         <v>10</v>
       </c>
       <c r="C127" t="n">
-        <v>0.04230484162395426</v>
+        <v>0.041963991076504836</v>
       </c>
     </row>
     <row r="128">
@@ -3512,7 +3512,7 @@
         <v>10</v>
       </c>
       <c r="C128" t="n">
-        <v>0.067797324202562</v>
+        <v>0.06690090028626293</v>
       </c>
     </row>
     <row r="129">
@@ -3523,7 +3523,7 @@
         <v>10</v>
       </c>
       <c r="C129" t="n">
-        <v>18.003928096220577</v>
+        <v>17.986221188736934</v>
       </c>
     </row>
     <row r="130">
@@ -3534,7 +3534,7 @@
         <v>10</v>
       </c>
       <c r="C130" t="n">
-        <v>16.99845752960712</v>
+        <v>17.05281731219263</v>
       </c>
     </row>
     <row r="131">
@@ -3545,7 +3545,7 @@
         <v>127</v>
       </c>
       <c r="C131" t="n">
-        <v>22298.850397398382</v>
+        <v>21004.044388035436</v>
       </c>
     </row>
     <row r="132">
@@ -3556,7 +3556,7 @@
         <v>127</v>
       </c>
       <c r="C132" t="n">
-        <v>18522.70009030306</v>
+        <v>15401.792908664305</v>
       </c>
     </row>
     <row r="133">
@@ -3567,7 +3567,7 @@
         <v>127</v>
       </c>
       <c r="C133" t="n">
-        <v>5834.421060878276</v>
+        <v>5780.908695859982</v>
       </c>
     </row>
     <row r="134">
@@ -3578,7 +3578,7 @@
         <v>127</v>
       </c>
       <c r="C134" t="n">
-        <v>5942.3694708622825</v>
+        <v>5888.69449134733</v>
       </c>
     </row>
     <row r="135">
@@ -3599,7 +3599,7 @@
         <v>19</v>
       </c>
       <c r="C137" t="n">
-        <v>353.00371411782953</v>
+        <v>371.01994774980994</v>
       </c>
     </row>
     <row r="138">
@@ -3610,7 +3610,7 @@
         <v>19</v>
       </c>
       <c r="C138" t="n">
-        <v>353.00371411782953</v>
+        <v>371.01994774980994</v>
       </c>
     </row>
     <row r="139">
@@ -3621,7 +3621,7 @@
         <v>10</v>
       </c>
       <c r="C139" t="n">
-        <v>0.5634841911382713</v>
+        <v>0.5922427067840472</v>
       </c>
     </row>
     <row r="140">
@@ -3632,7 +3632,7 @@
         <v>10</v>
       </c>
       <c r="C140" t="n">
-        <v>0.5634841911382713</v>
+        <v>0.5922427067840472</v>
       </c>
     </row>
     <row r="141">
@@ -3643,7 +3643,7 @@
         <v>10</v>
       </c>
       <c r="C141" t="n">
-        <v>0.34892378806167773</v>
+        <v>0.3126803878150592</v>
       </c>
     </row>
     <row r="142">
@@ -3654,7 +3654,7 @@
         <v>10</v>
       </c>
       <c r="C142" t="n">
-        <v>0.3423232528518342</v>
+        <v>0.30657970187675915</v>
       </c>
     </row>
     <row r="143">
@@ -3665,7 +3665,7 @@
         <v>10</v>
       </c>
       <c r="C143" t="n">
-        <v>0.029872272844491843</v>
+        <v>0.0293322744812582</v>
       </c>
     </row>
     <row r="144">
@@ -3676,7 +3676,7 @@
         <v>10</v>
       </c>
       <c r="C144" t="n">
-        <v>0.029767207654509704</v>
+        <v>0.0292561053992112</v>
       </c>
     </row>
     <row r="145">
@@ -3687,7 +3687,7 @@
         <v>10</v>
       </c>
       <c r="C145" t="n">
-        <v>11.68052360388158</v>
+        <v>10.659943469942835</v>
       </c>
     </row>
     <row r="146">
@@ -3698,7 +3698,7 @@
         <v>10</v>
       </c>
       <c r="C146" t="n">
-        <v>11.500012255935351</v>
+        <v>10.479169995232008</v>
       </c>
     </row>
     <row r="147">
@@ -3709,7 +3709,7 @@
         <v>127</v>
       </c>
       <c r="C147" t="n">
-        <v>8965.61573440322</v>
+        <v>9725.0885470675</v>
       </c>
     </row>
     <row r="148">
@@ -3720,7 +3720,7 @@
         <v>127</v>
       </c>
       <c r="C148" t="n">
-        <v>8955.0992076015</v>
+        <v>9721.600396203581</v>
       </c>
     </row>
     <row r="149">
@@ -3731,7 +3731,7 @@
         <v>127</v>
       </c>
       <c r="C149" t="n">
-        <v>8965.61573440322</v>
+        <v>9725.0885470675</v>
       </c>
     </row>
     <row r="150">
@@ -3742,7 +3742,7 @@
         <v>127</v>
       </c>
       <c r="C150" t="n">
-        <v>8955.0992076015</v>
+        <v>9721.600396203581</v>
       </c>
     </row>
     <row r="151">
@@ -3807,7 +3807,7 @@
         <v>10</v>
       </c>
       <c r="C157" t="n">
-        <v>0.5584166085349764</v>
+        <v>0.5525323981350044</v>
       </c>
     </row>
     <row r="158">
@@ -3818,7 +3818,7 @@
         <v>10</v>
       </c>
       <c r="C158" t="n">
-        <v>0.5561394717441098</v>
+        <v>0.5499384692056056</v>
       </c>
     </row>
     <row r="159">
@@ -3829,7 +3829,7 @@
         <v>10</v>
       </c>
       <c r="C159" t="n">
-        <v>0.03484624911605185</v>
+        <v>0.03465670567581535</v>
       </c>
     </row>
     <row r="160">
@@ -3840,7 +3840,7 @@
         <v>10</v>
       </c>
       <c r="C160" t="n">
-        <v>0.034772897500135465</v>
+        <v>0.03457314948397531</v>
       </c>
     </row>
     <row r="161">
@@ -3851,7 +3851,7 @@
         <v>10</v>
       </c>
       <c r="C161" t="n">
-        <v>16.02515687341921</v>
+        <v>15.943015568285265</v>
       </c>
     </row>
     <row r="162">
@@ -3862,7 +3862,7 @@
         <v>10</v>
       </c>
       <c r="C162" t="n">
-        <v>15.993475140860587</v>
+        <v>15.906519290656545</v>
       </c>
     </row>
     <row r="163">
@@ -3873,7 +3873,7 @@
         <v>127</v>
       </c>
       <c r="C163" t="n">
-        <v>662.675326948344</v>
+        <v>681.3310861812627</v>
       </c>
     </row>
     <row r="164">
@@ -3884,7 +3884,7 @@
         <v>127</v>
       </c>
       <c r="C164" t="n">
-        <v>-320.97531200747846</v>
+        <v>-186.678831898114</v>
       </c>
     </row>
     <row r="165">
@@ -3895,7 +3895,7 @@
         <v>127</v>
       </c>
       <c r="C165" t="n">
-        <v>6198.055528299885</v>
+        <v>6160.284105228036</v>
       </c>
     </row>
     <row r="166">
@@ -3906,7 +3906,7 @@
         <v>127</v>
       </c>
       <c r="C166" t="n">
-        <v>6183.43832543428</v>
+        <v>6143.6333772032385</v>
       </c>
     </row>
     <row r="167">
@@ -3971,7 +3971,7 @@
         <v>10</v>
       </c>
       <c r="C173" t="n">
-        <v>0.7240352555786533</v>
+        <v>0.7161677295041207</v>
       </c>
     </row>
     <row r="174">
@@ -3982,7 +3982,7 @@
         <v>10</v>
       </c>
       <c r="C174" t="n">
-        <v>0.7171881230077157</v>
+        <v>0.7093781988930395</v>
       </c>
     </row>
     <row r="175">
@@ -3993,7 +3993,7 @@
         <v>10</v>
       </c>
       <c r="C175" t="n">
-        <v>0.04118766769858103</v>
+        <v>0.04084117369444549</v>
       </c>
     </row>
     <row r="176">
@@ -4004,7 +4004,7 @@
         <v>10</v>
       </c>
       <c r="C176" t="n">
-        <v>0.04088611288212724</v>
+        <v>0.04054303166676981</v>
       </c>
     </row>
     <row r="177">
@@ -4015,7 +4015,7 @@
         <v>10</v>
       </c>
       <c r="C177" t="n">
-        <v>17.578933113602773</v>
+        <v>17.535434580361276</v>
       </c>
     </row>
     <row r="178">
@@ -4026,7 +4026,7 @@
         <v>10</v>
       </c>
       <c r="C178" t="n">
-        <v>17.541117813653152</v>
+        <v>17.49692042577234</v>
       </c>
     </row>
     <row r="179">
@@ -4037,7 +4037,7 @@
         <v>127</v>
       </c>
       <c r="C179" t="n">
-        <v>5877.131358722297</v>
+        <v>5827.689598819382</v>
       </c>
     </row>
     <row r="180">
@@ -4048,7 +4048,7 @@
         <v>127</v>
       </c>
       <c r="C180" t="n">
-        <v>5834.102040307761</v>
+        <v>5785.1472564602855</v>
       </c>
     </row>
     <row r="181">
@@ -4059,7 +4059,7 @@
         <v>127</v>
       </c>
       <c r="C181" t="n">
-        <v>5877.131358722297</v>
+        <v>5827.689598819382</v>
       </c>
     </row>
     <row r="182">
@@ -4070,7 +4070,7 @@
         <v>127</v>
       </c>
       <c r="C182" t="n">
-        <v>5834.102040307761</v>
+        <v>5785.1472564602855</v>
       </c>
     </row>
     <row r="183">
@@ -4135,7 +4135,7 @@
         <v>10</v>
       </c>
       <c r="C189" t="n">
-        <v>0.5496402939820478</v>
+        <v>0.5436505434948767</v>
       </c>
     </row>
     <row r="190">
@@ -4146,7 +4146,7 @@
         <v>10</v>
       </c>
       <c r="C190" t="n">
-        <v>0.54935857804511</v>
+        <v>0.5433529610748983</v>
       </c>
     </row>
     <row r="191">
@@ -4157,7 +4157,7 @@
         <v>10</v>
       </c>
       <c r="C191" t="n">
-        <v>0.03456354460008694</v>
+        <v>0.03437472069190256</v>
       </c>
     </row>
     <row r="192">
@@ -4168,7 +4168,7 @@
         <v>10</v>
       </c>
       <c r="C192" t="n">
-        <v>0.03455446990624919</v>
+        <v>0.034365602222511414</v>
       </c>
     </row>
     <row r="193">
@@ -4179,7 +4179,7 @@
         <v>10</v>
       </c>
       <c r="C193" t="n">
-        <v>15.902312692219226</v>
+        <v>15.815417043459531</v>
       </c>
     </row>
     <row r="194">
@@ -4190,7 +4190,7 @@
         <v>10</v>
       </c>
       <c r="C194" t="n">
-        <v>15.898336149725111</v>
+        <v>15.8109541499311</v>
       </c>
     </row>
     <row r="195">
@@ -4201,7 +4201,7 @@
         <v>127</v>
       </c>
       <c r="C195" t="n">
-        <v>-581.2712281829121</v>
+        <v>-535.6403424414048</v>
       </c>
     </row>
     <row r="196">
@@ -4212,7 +4212,7 @@
         <v>127</v>
       </c>
       <c r="C196" t="n">
-        <v>-732.6614086216566</v>
+        <v>-590.7377691701865</v>
       </c>
     </row>
     <row r="197">
@@ -4223,7 +4223,7 @@
         <v>127</v>
       </c>
       <c r="C197" t="n">
-        <v>6141.719356161671</v>
+        <v>6103.270459136028</v>
       </c>
     </row>
     <row r="198">
@@ -4234,7 +4234,7 @@
         <v>127</v>
       </c>
       <c r="C198" t="n">
-        <v>6139.910989173261</v>
+        <v>6101.360243368791</v>
       </c>
     </row>
     <row r="199">
@@ -4255,7 +4255,7 @@
         <v>19</v>
       </c>
       <c r="C201" t="n">
-        <v>120.05716075515801</v>
+        <v>119.39982458242625</v>
       </c>
     </row>
     <row r="202">
@@ -4277,7 +4277,7 @@
         <v>10</v>
       </c>
       <c r="C203" t="n">
-        <v>0.1815293997149729</v>
+        <v>0.1805354911459515</v>
       </c>
     </row>
     <row r="204">
@@ -4299,7 +4299,7 @@
         <v>10</v>
       </c>
       <c r="C205" t="n">
-        <v>1.8518202721030863</v>
+        <v>1.851820272103086</v>
       </c>
     </row>
     <row r="206">
@@ -4321,7 +4321,7 @@
         <v>10</v>
       </c>
       <c r="C207" t="n">
-        <v>0.21002130023993446</v>
+        <v>0.21002130023993443</v>
       </c>
     </row>
     <row r="208">
@@ -4365,7 +4365,7 @@
         <v>127</v>
       </c>
       <c r="C211" t="n">
-        <v>-2303.270047141946</v>
+        <v>-2283.0681038129965</v>
       </c>
     </row>
     <row r="212">
@@ -4387,7 +4387,7 @@
         <v>127</v>
       </c>
       <c r="C213" t="n">
-        <v>8998.357042534146</v>
+        <v>8900.057590043376</v>
       </c>
     </row>
     <row r="214">
@@ -4469,7 +4469,7 @@
         <v>53</v>
       </c>
       <c r="C6" t="n">
-        <v>1286.1942747218534</v>
+        <v>1078.4704390918146</v>
       </c>
     </row>
     <row r="7">
@@ -4534,7 +4534,7 @@
         <v>53</v>
       </c>
       <c r="C13" t="n">
-        <v>1286.1702208095278</v>
+        <v>1078.4518230487301</v>
       </c>
     </row>
     <row r="14">
@@ -4599,7 +4599,7 @@
         <v>53</v>
       </c>
       <c r="C20" t="n">
-        <v>2798.5356329150154</v>
+        <v>2579.2730386528165</v>
       </c>
     </row>
     <row r="21">
@@ -4659,7 +4659,7 @@
         <v>53</v>
       </c>
       <c r="C26" t="n">
-        <v>3112.981900989941</v>
+        <v>2959.8763165957816</v>
       </c>
     </row>
     <row r="27">

</xml_diff>